<commit_message>
added imu docs, updated time log and parts
</commit_message>
<xml_diff>
--- a/Documents/parts.xlsx
+++ b/Documents/parts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horia\Documents\COEN-6711\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43095294-A794-4A90-AF9F-114E512E7DEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7980DF80-4B7F-404A-9D4B-9A1C07B3724A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{7B036C92-D7F4-4C89-A46A-1E9A22510CC4}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>2-Wheel Self-Balancing Smart Robot Kit</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Adafruit Motor/Stepper/Servo Shield for Arduino v2 Kit - v2.3</t>
+  </si>
+  <si>
+    <t>https://abra-electronics.com/sensors/sensors-accelerometers-en/wave-100-10-dof-imu-sensor-low-power.html</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7590046-F8C1-406D-B636-76DB331AF851}">
-  <dimension ref="D4:D36"/>
+  <dimension ref="D4:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,6 +593,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>